<commit_message>
SQL for datyabase and updated readme
Create tables SQL and table design chanmge in xlsx, with reference to Trello page for managing tasks
</commit_message>
<xml_diff>
--- a/theme/AutoPoster database structure.xlsx
+++ b/theme/AutoPoster database structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Jonathan\Web\Spinning Monkey\git\spinningmonkey\theme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BDFB022-4C69-4933-A51B-21D357286A1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4CFC20-9A9A-4F0C-9AF7-C90CD336470E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2700" windowWidth="29040" windowHeight="15840" xr2:uid="{AB56387F-EC52-4BD4-AA3D-B2A52CAD2063}"/>
+    <workbookView xWindow="21480" yWindow="-2820" windowWidth="29040" windowHeight="15840" xr2:uid="{AB56387F-EC52-4BD4-AA3D-B2A52CAD2063}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">eg </t>
   </si>
@@ -92,9 +92,6 @@
     <t>The wordpress id of the auto generated post</t>
   </si>
   <si>
-    <t>INDEX</t>
-  </si>
-  <si>
     <t>The index of the article in the dynamically generated post</t>
   </si>
   <si>
@@ -117,6 +114,18 @@
   </si>
   <si>
     <t>0 means the post is only the summary text, image and hyperlink. 1 will mean we can skip it for processing - SQL query clause will only deal with entries where IS_EDITED is 0</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>CREATE TABLE `spinnis0_WPLXP`.`_LXP_auto_feed` ( `ID` BIGINT UNSIGNED NOT NULL AUTO_INCREMENT , `FEED` TEXT CHARACTER SET utf8mb4 COLLATE utf8mb4_unicode_520_ci NOT NULL , PRIMARY KEY (`ID`)) ENGINE = MyISAM CHARSET=utf8mb4 COLLATE utf8mb4_unicode_ci;</t>
+  </si>
+  <si>
+    <t>INDEX_IN_MARKUP</t>
+  </si>
+  <si>
+    <t>CREATE TABLE `spinnis0_WPLXP`.`LXP_auto_feed_posted` ( `AUTO_FEED_ID` BIGINT UNSIGNED NOT NULL , `POST_ID` BIGINT UNSIGNED NOT NULL , `INDEX_IN_MARKUP` INT UNSIGNED NOT NULL , `TITLE` VARCHAR(512) NOT NULL , `ORIGINAL_POST_HYPERLINK` VARCHAR(512) NOT NULL , `DATE_CREATED` DATETIME NOT NULL DEFAULT CURRENT_TIMESTAMP , `IS_EDITED` TINYINT(1) NOT NULL DEFAULT '0' , `NOTES` VARCHAR(512) NULL ) ENGINE = MyISAM;</t>
   </si>
 </sst>
 </file>
@@ -545,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6F651C-CA85-45E3-AE42-C70DC0EDDCF3}">
-  <dimension ref="B1:D16"/>
+  <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +567,7 @@
     <col min="4" max="4" width="95.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
@@ -568,8 +577,11 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
@@ -580,17 +592,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
     </row>
-    <row r="4" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -598,8 +610,11 @@
       <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
@@ -607,24 +622,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
@@ -635,20 +650,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4">
         <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>8</v>
@@ -657,7 +672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
@@ -668,7 +683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>7</v>
       </c>
@@ -677,7 +692,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>12</v>
       </c>
@@ -685,15 +700,18 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -701,5 +719,6 @@
     <hyperlink ref="C13" r:id="rId1" xr:uid="{DF0C1E1E-D916-4F0B-9E8B-FE661A0A9101}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create new log table for persisting log history
For every time the process writes new stuff, log that activity here if the page has the writelog parameter
</commit_message>
<xml_diff>
--- a/theme/AutoPoster database structure.xlsx
+++ b/theme/AutoPoster database structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Jonathan\Web\Spinning Monkey\git\spinningmonkey\theme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0984132C-02A8-44C8-A6F6-720C5ECC66C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1EABFB-FE0A-4D51-8356-C57088AD0537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2700" windowWidth="29040" windowHeight="15840" xr2:uid="{AB56387F-EC52-4BD4-AA3D-B2A52CAD2063}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t xml:space="preserve">eg </t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>CURRENT_LOG_TEXT</t>
+  </si>
+  <si>
+    <t>LAST_UPDATED</t>
   </si>
 </sst>
 </file>
@@ -566,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6F651C-CA85-45E3-AE42-C70DC0EDDCF3}">
-  <dimension ref="B1:E22"/>
+  <dimension ref="B1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +754,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C14" r:id="rId1" xr:uid="{DF0C1E1E-D916-4F0B-9E8B-FE661A0A9101}"/>

</xml_diff>